<commit_message>
update random generator excel (remove dot)
</commit_message>
<xml_diff>
--- a/events/2021-09-15/slides/乱数パスワード生成.xlsx
+++ b/events/2021-09-15/slides/乱数パスワード生成.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\tau\sproj\utelecon.github.io\events\2021-09-15\slides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C939D746-B1B5-482B-8AE3-457A0A093D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BCB818-66B0-4552-BD3A-E3D0F37822E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="1050" windowWidth="20775" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="14400" windowHeight="9945" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -82,10 +82,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ0123456789#$%&amp;()*+,-./:;&lt;=&gt;?@[]^_{|}~</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ0123456789</t>
   </si>
   <si>
@@ -277,6 +273,10 @@
     <rPh sb="24" eb="26">
       <t>コウシン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ0123456789#$%&amp;()*+,-/:;&lt;=&gt;?@[]^_{|}~</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -727,32 +727,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1">
         <f>LEN(B1)</f>
@@ -792,7 +792,7 @@
       </c>
       <c r="B2" s="2" t="str">
         <f ca="1">MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)</f>
-        <v>0AYolT45jJhiJ7f</v>
+        <v>YjjeAiBv9e1Kfa2</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">MID(C1,RANDBETWEEN(1,62),1)</f>
@@ -805,7 +805,7 @@
       </c>
       <c r="B3" s="3" t="str">
         <f ca="1">MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)</f>
-        <v>GzPGGgYCLpnhayV0PWaTQaQa597jyh</v>
+        <v>VCWfBPs2mmDPZqdlQlYEcNR8ZKfr0S</v>
       </c>
       <c r="C3" t="str">
         <f ca="1">MID(C2,RANDBETWEEN(1,62),1)</f>
@@ -818,7 +818,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f ca="1">MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)</f>
-        <v>bAtOhKbUIQyRRx67k1FrzLN0k2OknGlS3BpVhM2TdzaqT</v>
+        <v>4bjrVDP1upNIP2UKTB0OFeEafiCj0SDHDavTVOKXyTTJX</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -827,7 +827,7 @@
       </c>
       <c r="B5" s="4" t="str">
         <f ca="1">MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)</f>
-        <v>q1msieSc2udc3VkbU5noPAvkTRwNVRy6gPDy2HmCGVgHD1zgDiZBGbi1V5oR</v>
+        <v>JpH2iZ8TCbKiKX6TRjEuTEyyNsH9Ou4f3pKcbd2TJnEZLPjZ0FG28yUoZ6ga</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -838,7 +838,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -857,9 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -871,11 +869,11 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C1">
         <f>LEN(B1)</f>
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -884,7 +882,7 @@
       </c>
       <c r="B2" s="2" t="str">
         <f ca="1">MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)</f>
-        <v>dk_#rl*ifm=t.tL</v>
+        <v>|k^P&amp;f-4~=e68)R</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">MID(C1,RANDBETWEEN(1,62),1)</f>
@@ -897,7 +895,7 @@
       </c>
       <c r="B3" s="3" t="str">
         <f ca="1">MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)</f>
-        <v>ZX8Lqj$W2:B?~NVAv7?tC]nQ$7_Y)V</v>
+        <v>J~w[FJ|plF(|An,/N&lt;j2b@7S5iVm*9</v>
       </c>
       <c r="C3" t="str">
         <f ca="1">MID(C2,RANDBETWEEN(1,62),1)</f>
@@ -910,7 +908,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f ca="1">MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)</f>
-        <v>#$9)a.K&gt;ULNq&amp;1DfZ(WfGf}seZND*nuNV#-9%c$g=dnzz</v>
+        <v>T3,NBG)+I}AIT|xrFh1o-&lt;0~W?0-3%E?m6_R1kdIbZGHP</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -919,7 +917,7 @@
       </c>
       <c r="B5" s="4" t="str">
         <f ca="1">MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)&amp;MID($B$1,RANDBETWEEN(1,$C$1),1)</f>
-        <v>ylr&lt;nwNIAy~XVMdWdAD)3DnpNPO.p&gt;&amp;H2t(iLLNmCv|+Qg-MPqPqG{+*^EPp</v>
+        <v>7bF_C{yxHK&gt;:TJ@~PXq8YtngbG_Qra$py]:C#{N7tZM=d$&amp;GUg0maQM8EsgY</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -930,7 +928,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>